<commit_message>
minor cosmetics and id
</commit_message>
<xml_diff>
--- a/hw1/giladsol/Ass-1 Tables.xlsx
+++ b/hw1/giladsol/Ass-1 Tables.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17426"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Q1" sheetId="1" r:id="rId1"/>
     <sheet name="Q2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -167,15 +167,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="8">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="166" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="167" formatCode="0.000"/>
     <numFmt numFmtId="168" formatCode="&quot;$&quot;#,##0.000"/>
-    <numFmt numFmtId="169" formatCode="_ * #,##0.0_ ;_ * \-#,##0.0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="170" formatCode="_ * #,##0.000_ ;_ * \-#,##0.000_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="171" formatCode="0.0000"/>
   </numFmts>
@@ -502,11 +501,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -583,9 +583,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -634,28 +631,13 @@
     <xf numFmtId="168" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="3" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="168" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="3" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="168" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -664,12 +646,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -698,6 +674,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -757,22 +739,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="0" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="3" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -821,7 +819,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -854,9 +852,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -889,6 +904,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1067,8 +1099,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:S37"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12:P13"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O19" sqref="O19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1084,12 +1116,12 @@
     <col min="9" max="9" width="7.75" style="7" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.5" style="7" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15.5" style="7" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.125" style="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.875" style="7" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="6.875" style="7" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="7.75" style="7" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="9.875" style="7" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="15.5" style="7" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8.875" style="7" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.5" style="7" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="13.5" style="7" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="16.5" style="7" bestFit="1" customWidth="1"/>
     <col min="20" max="16384" width="7.875" style="7"/>
@@ -1108,30 +1140,30 @@
     </row>
     <row r="3" spans="1:19" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" s="5"/>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="65" t="s">
+      <c r="C3" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="66"/>
-      <c r="E3" s="66"/>
-      <c r="F3" s="66"/>
-      <c r="G3" s="67"/>
-      <c r="H3" s="65" t="s">
+      <c r="D3" s="60"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="60"/>
+      <c r="G3" s="61"/>
+      <c r="H3" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="66"/>
-      <c r="J3" s="66"/>
-      <c r="K3" s="66"/>
-      <c r="L3" s="67"/>
-      <c r="M3" s="65" t="s">
+      <c r="I3" s="60"/>
+      <c r="J3" s="60"/>
+      <c r="K3" s="60"/>
+      <c r="L3" s="61"/>
+      <c r="M3" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="N3" s="66"/>
-      <c r="O3" s="66"/>
-      <c r="P3" s="66"/>
-      <c r="Q3" s="67"/>
+      <c r="N3" s="60"/>
+      <c r="O3" s="60"/>
+      <c r="P3" s="60"/>
+      <c r="Q3" s="61"/>
       <c r="R3" s="17"/>
       <c r="S3" s="13"/>
     </row>
@@ -1192,609 +1224,611 @@
     </row>
     <row r="5" spans="1:19" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="10"/>
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="28" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="21">
         <v>23.87</v>
       </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="33"/>
+      <c r="D5" s="78"/>
+      <c r="E5" s="32"/>
       <c r="F5" s="11"/>
       <c r="G5" s="22"/>
       <c r="H5" s="21">
         <v>84.65</v>
       </c>
-      <c r="I5" s="1"/>
-      <c r="J5" s="33"/>
+      <c r="I5" s="78"/>
+      <c r="J5" s="32"/>
       <c r="K5" s="11"/>
       <c r="L5" s="22"/>
-      <c r="M5" s="21">
+      <c r="M5" s="42">
         <v>33.200000000000003</v>
       </c>
-      <c r="N5" s="1"/>
-      <c r="O5" s="33"/>
+      <c r="N5" s="78"/>
+      <c r="O5" s="32"/>
       <c r="P5" s="11"/>
       <c r="Q5" s="22"/>
-      <c r="R5" s="31"/>
-      <c r="S5" s="51">
+      <c r="R5" s="30"/>
+      <c r="S5" s="45">
         <v>670980000</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="10"/>
-      <c r="B6" s="30"/>
+      <c r="B6" s="29"/>
       <c r="C6" s="23"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="43">
+      <c r="D6" s="79"/>
+      <c r="E6" s="31">
         <v>11243904</v>
       </c>
-      <c r="F6" s="42">
+      <c r="F6" s="41">
         <f>E6*C5</f>
         <v>268391988.48000002</v>
       </c>
       <c r="G6" s="24"/>
       <c r="H6" s="23"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="32">
+      <c r="I6" s="79"/>
+      <c r="J6" s="31">
         <v>2774282</v>
       </c>
-      <c r="K6" s="42">
+      <c r="K6" s="41">
         <f>J6*H5</f>
         <v>234842971.30000001</v>
       </c>
       <c r="L6" s="24"/>
-      <c r="M6" s="23"/>
-      <c r="N6" s="13"/>
-      <c r="O6" s="32">
+      <c r="M6" s="82"/>
+      <c r="N6" s="79"/>
+      <c r="O6" s="31">
         <v>5052560</v>
       </c>
-      <c r="P6" s="42">
+      <c r="P6" s="41">
         <f>M5*O6</f>
         <v>167744992</v>
       </c>
       <c r="Q6" s="24"/>
-      <c r="R6" s="53">
+      <c r="R6" s="83">
         <f>S5-(P6+K6+F6)</f>
         <v>48.220000028610229</v>
       </c>
-      <c r="S6" s="42">
+      <c r="S6" s="41">
         <f>P6+R6+K6+F6</f>
         <v>670980000</v>
       </c>
     </row>
     <row r="7" spans="1:19" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="10"/>
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="45">
+      <c r="C7" s="42">
         <f>C5*(1+D7)</f>
         <v>24.428558000000002</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="78">
         <v>2.3400000000000001E-2</v>
       </c>
-      <c r="E7" s="50">
+      <c r="E7" s="32">
         <f>E6-G6</f>
         <v>11243904</v>
       </c>
-      <c r="F7" s="51">
+      <c r="F7" s="45">
         <f>C7*E7</f>
         <v>274672361.010432</v>
       </c>
-      <c r="G7" s="44">
+      <c r="G7" s="81">
         <f>E7 - FLOOR((E2*$S$7)/C7,1)</f>
         <v>168757</v>
       </c>
-      <c r="H7" s="46">
+      <c r="H7" s="42">
         <f>H5*(1+I7)</f>
         <v>86.114445000000018</v>
       </c>
-      <c r="I7" s="1">
+      <c r="I7" s="78">
         <v>1.7299999999999999E-2</v>
       </c>
-      <c r="J7" s="33">
+      <c r="J7" s="32">
         <f>J6-L6</f>
         <v>2774282</v>
       </c>
-      <c r="K7" s="51">
+      <c r="K7" s="45">
         <f>J7*H7</f>
         <v>238905754.70349005</v>
       </c>
-      <c r="L7" s="22">
+      <c r="L7" s="81">
         <f>J7 - FLOOR((J2*$S$7)/H7,1)</f>
         <v>25253</v>
       </c>
-      <c r="M7" s="45">
+      <c r="M7" s="42">
         <f>M5*(1+N7)</f>
         <v>32.220600000000005</v>
       </c>
-      <c r="N7" s="1">
+      <c r="N7" s="78">
         <v>-2.9499999999999998E-2</v>
       </c>
-      <c r="O7" s="33">
+      <c r="O7" s="32">
         <f>O6-Q6</f>
         <v>5052560</v>
       </c>
-      <c r="P7" s="51">
+      <c r="P7" s="45">
         <f>M7*O7</f>
         <v>162796514.73600003</v>
       </c>
-      <c r="Q7" s="22">
+      <c r="Q7" s="81">
         <f>O7 - FLOOR((O2*$S$7)/M7,1)</f>
         <v>-195438</v>
       </c>
-      <c r="R7" s="54">
+      <c r="R7" s="30">
         <v>48.220000028610229</v>
       </c>
-      <c r="S7" s="51">
+      <c r="S7" s="45">
         <f t="shared" ref="S7:S10" si="0">P7+R7+K7+F7</f>
         <v>676374678.66992211</v>
       </c>
     </row>
     <row r="8" spans="1:19" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="10"/>
-      <c r="B8" s="30"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="43">
+      <c r="B8" s="29"/>
+      <c r="C8" s="82"/>
+      <c r="D8" s="79"/>
+      <c r="E8" s="31">
         <f>E7-G7</f>
         <v>11075147</v>
       </c>
-      <c r="F8" s="42">
+      <c r="F8" s="41">
         <f>C7*E8</f>
         <v>270549870.84802604</v>
       </c>
       <c r="G8" s="24"/>
       <c r="H8" s="23"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="32">
+      <c r="I8" s="79"/>
+      <c r="J8" s="31">
         <f>J7-L7</f>
         <v>2749029</v>
       </c>
-      <c r="K8" s="42">
+      <c r="K8" s="41">
         <f>H7*J8</f>
         <v>236731106.62390506</v>
       </c>
       <c r="L8" s="24"/>
-      <c r="M8" s="23"/>
-      <c r="N8" s="13"/>
-      <c r="O8" s="32">
+      <c r="M8" s="82"/>
+      <c r="N8" s="79"/>
+      <c r="O8" s="31">
         <f>O7-Q7</f>
         <v>5247998</v>
       </c>
-      <c r="P8" s="42">
+      <c r="P8" s="41">
         <f>M7*O8</f>
         <v>169093644.35880002</v>
       </c>
       <c r="Q8" s="24"/>
-      <c r="R8" s="53">
+      <c r="R8" s="83">
         <f>S7-P8-K8-F8</f>
         <v>56.83919095993042</v>
       </c>
-      <c r="S8" s="42">
+      <c r="S8" s="41">
         <f t="shared" si="0"/>
         <v>676374678.66992211</v>
       </c>
     </row>
     <row r="9" spans="1:19" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="10"/>
-      <c r="B9" s="29" t="s">
+      <c r="B9" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="45">
+      <c r="C9" s="42">
         <f t="shared" ref="C9" si="1">C7*(1+D9)</f>
         <v>23.378130006000003</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="78">
         <v>-4.2999999999999997E-2</v>
       </c>
-      <c r="E9" s="50">
+      <c r="E9" s="32">
         <f>E8</f>
         <v>11075147</v>
       </c>
-      <c r="F9" s="51">
+      <c r="F9" s="45">
         <f>C9*E9</f>
         <v>258916226.4015609</v>
       </c>
-      <c r="G9" s="44">
+      <c r="G9" s="81">
         <f>E9 - FLOOR((E2*$S$9)/C9,1)</f>
         <v>-387630</v>
       </c>
-      <c r="H9" s="46">
+      <c r="H9" s="42">
         <f>H7*(1+I9)</f>
         <v>87.208098451500007</v>
       </c>
-      <c r="I9" s="1">
+      <c r="I9" s="78">
         <v>1.2699999999999999E-2</v>
       </c>
-      <c r="J9" s="33">
+      <c r="J9" s="32">
         <f>J8</f>
         <v>2749029</v>
       </c>
-      <c r="K9" s="51">
+      <c r="K9" s="45">
         <f>J9*H9</f>
         <v>239737591.67802861</v>
       </c>
-      <c r="L9" s="22">
+      <c r="L9" s="81">
         <f>J9 - FLOOR((J2*$S$9)/H9,1)</f>
         <v>60277</v>
       </c>
-      <c r="M9" s="45">
+      <c r="M9" s="42">
         <f>M7*(1+N9)</f>
         <v>32.639467799999998</v>
       </c>
-      <c r="N9" s="1">
+      <c r="N9" s="78">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="O9" s="33">
+      <c r="O9" s="32">
         <f>O8</f>
         <v>5247998</v>
       </c>
-      <c r="P9" s="51">
+      <c r="P9" s="45">
         <f>M9*O9</f>
         <v>171291861.73546439</v>
       </c>
-      <c r="Q9" s="22">
+      <c r="Q9" s="81">
         <f>O9 - FLOOR((O2*$S$9)/M9,1)</f>
         <v>116590</v>
       </c>
-      <c r="R9" s="54">
+      <c r="R9" s="30">
         <f>R8</f>
         <v>56.83919095993042</v>
       </c>
-      <c r="S9" s="51">
+      <c r="S9" s="45">
         <f t="shared" si="0"/>
         <v>669945736.6542449</v>
       </c>
     </row>
     <row r="10" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12"/>
-      <c r="B10" s="30"/>
+      <c r="B10" s="29"/>
       <c r="C10" s="25"/>
-      <c r="D10" s="26"/>
-      <c r="E10" s="47">
+      <c r="D10" s="80"/>
+      <c r="E10" s="44">
         <f>E9-G9</f>
         <v>11462777</v>
       </c>
-      <c r="F10" s="48">
+      <c r="F10" s="43">
         <f>C9*E10</f>
         <v>267978290.93578669</v>
       </c>
-      <c r="G10" s="27"/>
+      <c r="G10" s="26"/>
       <c r="H10" s="25"/>
-      <c r="I10" s="26"/>
-      <c r="J10" s="49">
+      <c r="I10" s="80"/>
+      <c r="J10" s="44">
         <f>J9-L9</f>
         <v>2688752</v>
       </c>
-      <c r="K10" s="48">
+      <c r="K10" s="43">
         <f>H9*J10</f>
         <v>234480949.12766755</v>
       </c>
-      <c r="L10" s="27"/>
+      <c r="L10" s="26"/>
       <c r="M10" s="25"/>
-      <c r="N10" s="26"/>
-      <c r="O10" s="49">
+      <c r="N10" s="80"/>
+      <c r="O10" s="44">
         <f>O9-Q9</f>
         <v>5131408</v>
       </c>
-      <c r="P10" s="48">
+      <c r="P10" s="43">
         <f>M9*O10</f>
         <v>167486426.1846624</v>
       </c>
-      <c r="Q10" s="27"/>
-      <c r="R10" s="53">
+      <c r="Q10" s="26"/>
+      <c r="R10" s="83">
         <f>S9-P10-K10-F10</f>
         <v>70.406128257513046</v>
       </c>
-      <c r="S10" s="42">
+      <c r="S10" s="41">
         <f t="shared" si="0"/>
         <v>669945736.6542449</v>
       </c>
     </row>
     <row r="11" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="68" t="s">
+      <c r="B12" s="62" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="69"/>
-      <c r="D12" s="69"/>
-      <c r="E12" s="69"/>
-      <c r="F12" s="69"/>
-      <c r="G12" s="69"/>
-      <c r="H12" s="69"/>
-      <c r="I12" s="70"/>
-      <c r="O12" s="84" t="s">
+      <c r="C12" s="63"/>
+      <c r="D12" s="63"/>
+      <c r="E12" s="63"/>
+      <c r="F12" s="63"/>
+      <c r="G12" s="63"/>
+      <c r="H12" s="63"/>
+      <c r="I12" s="64"/>
+      <c r="O12" s="57" t="s">
         <v>36</v>
       </c>
-      <c r="P12" s="85" t="s">
+      <c r="P12" s="58" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B13" s="71"/>
-      <c r="C13" s="72"/>
-      <c r="D13" s="72"/>
-      <c r="E13" s="72"/>
-      <c r="F13" s="72"/>
-      <c r="G13" s="72"/>
-      <c r="H13" s="72"/>
-      <c r="I13" s="73"/>
-      <c r="O13" s="85"/>
-      <c r="P13" s="85" t="s">
+      <c r="B13" s="65"/>
+      <c r="C13" s="66"/>
+      <c r="D13" s="66"/>
+      <c r="E13" s="66"/>
+      <c r="F13" s="66"/>
+      <c r="G13" s="66"/>
+      <c r="H13" s="66"/>
+      <c r="I13" s="67"/>
+      <c r="O13" s="58">
+        <v>306555822</v>
+      </c>
+      <c r="P13" s="58" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B14" s="71"/>
-      <c r="C14" s="72"/>
-      <c r="D14" s="72"/>
-      <c r="E14" s="72"/>
-      <c r="F14" s="72"/>
-      <c r="G14" s="72"/>
-      <c r="H14" s="72"/>
-      <c r="I14" s="73"/>
-      <c r="J14" s="41"/>
+      <c r="B14" s="65"/>
+      <c r="C14" s="66"/>
+      <c r="D14" s="66"/>
+      <c r="E14" s="66"/>
+      <c r="F14" s="66"/>
+      <c r="G14" s="66"/>
+      <c r="H14" s="66"/>
+      <c r="I14" s="67"/>
+      <c r="J14" s="40"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B15" s="71"/>
-      <c r="C15" s="72"/>
-      <c r="D15" s="72"/>
-      <c r="E15" s="72"/>
-      <c r="F15" s="72"/>
-      <c r="G15" s="72"/>
-      <c r="H15" s="72"/>
-      <c r="I15" s="73"/>
-      <c r="K15" s="55"/>
+      <c r="B15" s="65"/>
+      <c r="C15" s="66"/>
+      <c r="D15" s="66"/>
+      <c r="E15" s="66"/>
+      <c r="F15" s="66"/>
+      <c r="G15" s="66"/>
+      <c r="H15" s="66"/>
+      <c r="I15" s="67"/>
+      <c r="K15" s="47"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B16" s="71"/>
-      <c r="C16" s="72"/>
-      <c r="D16" s="72"/>
-      <c r="E16" s="72"/>
-      <c r="F16" s="72"/>
-      <c r="G16" s="72"/>
-      <c r="H16" s="72"/>
-      <c r="I16" s="73"/>
-      <c r="J16" s="41"/>
-      <c r="K16" s="41"/>
+      <c r="B16" s="65"/>
+      <c r="C16" s="66"/>
+      <c r="D16" s="66"/>
+      <c r="E16" s="66"/>
+      <c r="F16" s="66"/>
+      <c r="G16" s="66"/>
+      <c r="H16" s="66"/>
+      <c r="I16" s="67"/>
+      <c r="J16" s="40"/>
+      <c r="K16" s="40"/>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B17" s="71"/>
-      <c r="C17" s="72"/>
-      <c r="D17" s="72"/>
-      <c r="E17" s="72"/>
-      <c r="F17" s="72"/>
-      <c r="G17" s="72"/>
-      <c r="H17" s="72"/>
-      <c r="I17" s="73"/>
-      <c r="J17" s="41"/>
-      <c r="K17" s="56"/>
+      <c r="B17" s="65"/>
+      <c r="C17" s="66"/>
+      <c r="D17" s="66"/>
+      <c r="E17" s="66"/>
+      <c r="F17" s="66"/>
+      <c r="G17" s="66"/>
+      <c r="H17" s="66"/>
+      <c r="I17" s="67"/>
+      <c r="J17" s="40"/>
+      <c r="K17" s="48"/>
     </row>
     <row r="18" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="74"/>
-      <c r="C18" s="75"/>
-      <c r="D18" s="75"/>
-      <c r="E18" s="75"/>
-      <c r="F18" s="75"/>
-      <c r="G18" s="75"/>
-      <c r="H18" s="75"/>
-      <c r="I18" s="76"/>
+      <c r="B18" s="68"/>
+      <c r="C18" s="69"/>
+      <c r="D18" s="69"/>
+      <c r="E18" s="69"/>
+      <c r="F18" s="69"/>
+      <c r="G18" s="69"/>
+      <c r="H18" s="69"/>
+      <c r="I18" s="70"/>
     </row>
     <row r="19" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="52"/>
-      <c r="C19" s="52"/>
-      <c r="D19" s="52"/>
-      <c r="E19" s="52"/>
-      <c r="F19" s="52"/>
-      <c r="G19" s="52"/>
-      <c r="H19" s="52"/>
-      <c r="I19" s="52"/>
+      <c r="B19" s="46"/>
+      <c r="C19" s="46"/>
+      <c r="D19" s="46"/>
+      <c r="E19" s="46"/>
+      <c r="F19" s="46"/>
+      <c r="G19" s="46"/>
+      <c r="H19" s="46"/>
+      <c r="I19" s="46"/>
     </row>
     <row r="20" spans="2:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="68" t="s">
+      <c r="B20" s="62" t="s">
         <v>29</v>
       </c>
-      <c r="C20" s="69"/>
-      <c r="D20" s="69"/>
-      <c r="E20" s="69"/>
-      <c r="F20" s="69"/>
-      <c r="G20" s="69"/>
-      <c r="H20" s="69"/>
-      <c r="I20" s="69"/>
-      <c r="J20" s="70"/>
+      <c r="C20" s="63"/>
+      <c r="D20" s="63"/>
+      <c r="E20" s="63"/>
+      <c r="F20" s="63"/>
+      <c r="G20" s="63"/>
+      <c r="H20" s="63"/>
+      <c r="I20" s="63"/>
+      <c r="J20" s="64"/>
     </row>
     <row r="21" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B21" s="71"/>
-      <c r="C21" s="72"/>
-      <c r="D21" s="72"/>
-      <c r="E21" s="72"/>
-      <c r="F21" s="72"/>
-      <c r="G21" s="72"/>
-      <c r="H21" s="72"/>
-      <c r="I21" s="72"/>
-      <c r="J21" s="73"/>
-      <c r="K21" s="55"/>
-      <c r="R21" s="57"/>
+      <c r="B21" s="65"/>
+      <c r="C21" s="66"/>
+      <c r="D21" s="66"/>
+      <c r="E21" s="66"/>
+      <c r="F21" s="66"/>
+      <c r="G21" s="66"/>
+      <c r="H21" s="66"/>
+      <c r="I21" s="66"/>
+      <c r="J21" s="67"/>
+      <c r="K21" s="47"/>
+      <c r="R21" s="49"/>
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B22" s="71"/>
-      <c r="C22" s="72"/>
-      <c r="D22" s="72"/>
-      <c r="E22" s="72"/>
-      <c r="F22" s="72"/>
-      <c r="G22" s="72"/>
-      <c r="H22" s="72"/>
-      <c r="I22" s="72"/>
-      <c r="J22" s="73"/>
-      <c r="R22" s="55"/>
+      <c r="B22" s="65"/>
+      <c r="C22" s="66"/>
+      <c r="D22" s="66"/>
+      <c r="E22" s="66"/>
+      <c r="F22" s="66"/>
+      <c r="G22" s="66"/>
+      <c r="H22" s="66"/>
+      <c r="I22" s="66"/>
+      <c r="J22" s="67"/>
+      <c r="R22" s="47"/>
     </row>
     <row r="23" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B23" s="71"/>
-      <c r="C23" s="72"/>
-      <c r="D23" s="72"/>
-      <c r="E23" s="72"/>
-      <c r="F23" s="72"/>
-      <c r="G23" s="72"/>
-      <c r="H23" s="72"/>
-      <c r="I23" s="72"/>
-      <c r="J23" s="73"/>
+      <c r="B23" s="65"/>
+      <c r="C23" s="66"/>
+      <c r="D23" s="66"/>
+      <c r="E23" s="66"/>
+      <c r="F23" s="66"/>
+      <c r="G23" s="66"/>
+      <c r="H23" s="66"/>
+      <c r="I23" s="66"/>
+      <c r="J23" s="67"/>
     </row>
     <row r="24" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B24" s="71"/>
-      <c r="C24" s="72"/>
-      <c r="D24" s="72"/>
-      <c r="E24" s="72"/>
-      <c r="F24" s="72"/>
-      <c r="G24" s="72"/>
-      <c r="H24" s="72"/>
-      <c r="I24" s="72"/>
-      <c r="J24" s="73"/>
+      <c r="B24" s="65"/>
+      <c r="C24" s="66"/>
+      <c r="D24" s="66"/>
+      <c r="E24" s="66"/>
+      <c r="F24" s="66"/>
+      <c r="G24" s="66"/>
+      <c r="H24" s="66"/>
+      <c r="I24" s="66"/>
+      <c r="J24" s="67"/>
     </row>
     <row r="25" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B25" s="71"/>
-      <c r="C25" s="72"/>
-      <c r="D25" s="72"/>
-      <c r="E25" s="72"/>
-      <c r="F25" s="72"/>
-      <c r="G25" s="72"/>
-      <c r="H25" s="72"/>
-      <c r="I25" s="72"/>
-      <c r="J25" s="73"/>
+      <c r="B25" s="65"/>
+      <c r="C25" s="66"/>
+      <c r="D25" s="66"/>
+      <c r="E25" s="66"/>
+      <c r="F25" s="66"/>
+      <c r="G25" s="66"/>
+      <c r="H25" s="66"/>
+      <c r="I25" s="66"/>
+      <c r="J25" s="67"/>
     </row>
     <row r="26" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B26" s="71"/>
-      <c r="C26" s="72"/>
-      <c r="D26" s="72"/>
-      <c r="E26" s="72"/>
-      <c r="F26" s="72"/>
-      <c r="G26" s="72"/>
-      <c r="H26" s="72"/>
-      <c r="I26" s="72"/>
-      <c r="J26" s="73"/>
+      <c r="B26" s="65"/>
+      <c r="C26" s="66"/>
+      <c r="D26" s="66"/>
+      <c r="E26" s="66"/>
+      <c r="F26" s="66"/>
+      <c r="G26" s="66"/>
+      <c r="H26" s="66"/>
+      <c r="I26" s="66"/>
+      <c r="J26" s="67"/>
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B27" s="71"/>
-      <c r="C27" s="72"/>
-      <c r="D27" s="72"/>
-      <c r="E27" s="72"/>
-      <c r="F27" s="72"/>
-      <c r="G27" s="72"/>
-      <c r="H27" s="72"/>
-      <c r="I27" s="72"/>
-      <c r="J27" s="73"/>
+      <c r="B27" s="65"/>
+      <c r="C27" s="66"/>
+      <c r="D27" s="66"/>
+      <c r="E27" s="66"/>
+      <c r="F27" s="66"/>
+      <c r="G27" s="66"/>
+      <c r="H27" s="66"/>
+      <c r="I27" s="66"/>
+      <c r="J27" s="67"/>
     </row>
     <row r="28" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B28" s="71"/>
-      <c r="C28" s="72"/>
-      <c r="D28" s="72"/>
-      <c r="E28" s="72"/>
-      <c r="F28" s="72"/>
-      <c r="G28" s="72"/>
-      <c r="H28" s="72"/>
-      <c r="I28" s="72"/>
-      <c r="J28" s="73"/>
+      <c r="B28" s="65"/>
+      <c r="C28" s="66"/>
+      <c r="D28" s="66"/>
+      <c r="E28" s="66"/>
+      <c r="F28" s="66"/>
+      <c r="G28" s="66"/>
+      <c r="H28" s="66"/>
+      <c r="I28" s="66"/>
+      <c r="J28" s="67"/>
     </row>
     <row r="29" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B29" s="71"/>
-      <c r="C29" s="72"/>
-      <c r="D29" s="72"/>
-      <c r="E29" s="72"/>
-      <c r="F29" s="72"/>
-      <c r="G29" s="72"/>
-      <c r="H29" s="72"/>
-      <c r="I29" s="72"/>
-      <c r="J29" s="73"/>
+      <c r="B29" s="65"/>
+      <c r="C29" s="66"/>
+      <c r="D29" s="66"/>
+      <c r="E29" s="66"/>
+      <c r="F29" s="66"/>
+      <c r="G29" s="66"/>
+      <c r="H29" s="66"/>
+      <c r="I29" s="66"/>
+      <c r="J29" s="67"/>
     </row>
     <row r="30" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B30" s="71"/>
-      <c r="C30" s="72"/>
-      <c r="D30" s="72"/>
-      <c r="E30" s="72"/>
-      <c r="F30" s="72"/>
-      <c r="G30" s="72"/>
-      <c r="H30" s="72"/>
-      <c r="I30" s="72"/>
-      <c r="J30" s="73"/>
+      <c r="B30" s="65"/>
+      <c r="C30" s="66"/>
+      <c r="D30" s="66"/>
+      <c r="E30" s="66"/>
+      <c r="F30" s="66"/>
+      <c r="G30" s="66"/>
+      <c r="H30" s="66"/>
+      <c r="I30" s="66"/>
+      <c r="J30" s="67"/>
     </row>
     <row r="31" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B31" s="71"/>
-      <c r="C31" s="72"/>
-      <c r="D31" s="72"/>
-      <c r="E31" s="72"/>
-      <c r="F31" s="72"/>
-      <c r="G31" s="72"/>
-      <c r="H31" s="72"/>
-      <c r="I31" s="72"/>
-      <c r="J31" s="73"/>
+      <c r="B31" s="65"/>
+      <c r="C31" s="66"/>
+      <c r="D31" s="66"/>
+      <c r="E31" s="66"/>
+      <c r="F31" s="66"/>
+      <c r="G31" s="66"/>
+      <c r="H31" s="66"/>
+      <c r="I31" s="66"/>
+      <c r="J31" s="67"/>
     </row>
     <row r="32" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B32" s="71"/>
-      <c r="C32" s="72"/>
-      <c r="D32" s="72"/>
-      <c r="E32" s="72"/>
-      <c r="F32" s="72"/>
-      <c r="G32" s="72"/>
-      <c r="H32" s="72"/>
-      <c r="I32" s="72"/>
-      <c r="J32" s="73"/>
+      <c r="B32" s="65"/>
+      <c r="C32" s="66"/>
+      <c r="D32" s="66"/>
+      <c r="E32" s="66"/>
+      <c r="F32" s="66"/>
+      <c r="G32" s="66"/>
+      <c r="H32" s="66"/>
+      <c r="I32" s="66"/>
+      <c r="J32" s="67"/>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B33" s="71"/>
-      <c r="C33" s="72"/>
-      <c r="D33" s="72"/>
-      <c r="E33" s="72"/>
-      <c r="F33" s="72"/>
-      <c r="G33" s="72"/>
-      <c r="H33" s="72"/>
-      <c r="I33" s="72"/>
-      <c r="J33" s="73"/>
+      <c r="B33" s="65"/>
+      <c r="C33" s="66"/>
+      <c r="D33" s="66"/>
+      <c r="E33" s="66"/>
+      <c r="F33" s="66"/>
+      <c r="G33" s="66"/>
+      <c r="H33" s="66"/>
+      <c r="I33" s="66"/>
+      <c r="J33" s="67"/>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B34" s="71"/>
-      <c r="C34" s="72"/>
-      <c r="D34" s="72"/>
-      <c r="E34" s="72"/>
-      <c r="F34" s="72"/>
-      <c r="G34" s="72"/>
-      <c r="H34" s="72"/>
-      <c r="I34" s="72"/>
-      <c r="J34" s="73"/>
+      <c r="B34" s="65"/>
+      <c r="C34" s="66"/>
+      <c r="D34" s="66"/>
+      <c r="E34" s="66"/>
+      <c r="F34" s="66"/>
+      <c r="G34" s="66"/>
+      <c r="H34" s="66"/>
+      <c r="I34" s="66"/>
+      <c r="J34" s="67"/>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B35" s="71"/>
-      <c r="C35" s="72"/>
-      <c r="D35" s="72"/>
-      <c r="E35" s="72"/>
-      <c r="F35" s="72"/>
-      <c r="G35" s="72"/>
-      <c r="H35" s="72"/>
-      <c r="I35" s="72"/>
-      <c r="J35" s="73"/>
+      <c r="B35" s="65"/>
+      <c r="C35" s="66"/>
+      <c r="D35" s="66"/>
+      <c r="E35" s="66"/>
+      <c r="F35" s="66"/>
+      <c r="G35" s="66"/>
+      <c r="H35" s="66"/>
+      <c r="I35" s="66"/>
+      <c r="J35" s="67"/>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B36" s="71"/>
-      <c r="C36" s="72"/>
-      <c r="D36" s="72"/>
-      <c r="E36" s="72"/>
-      <c r="F36" s="72"/>
-      <c r="G36" s="72"/>
-      <c r="H36" s="72"/>
-      <c r="I36" s="72"/>
-      <c r="J36" s="73"/>
+      <c r="B36" s="65"/>
+      <c r="C36" s="66"/>
+      <c r="D36" s="66"/>
+      <c r="E36" s="66"/>
+      <c r="F36" s="66"/>
+      <c r="G36" s="66"/>
+      <c r="H36" s="66"/>
+      <c r="I36" s="66"/>
+      <c r="J36" s="67"/>
     </row>
     <row r="37" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="74"/>
-      <c r="C37" s="75"/>
-      <c r="D37" s="75"/>
-      <c r="E37" s="75"/>
-      <c r="F37" s="75"/>
-      <c r="G37" s="75"/>
-      <c r="H37" s="75"/>
-      <c r="I37" s="75"/>
-      <c r="J37" s="76"/>
+      <c r="B37" s="68"/>
+      <c r="C37" s="69"/>
+      <c r="D37" s="69"/>
+      <c r="E37" s="69"/>
+      <c r="F37" s="69"/>
+      <c r="G37" s="69"/>
+      <c r="H37" s="69"/>
+      <c r="I37" s="69"/>
+      <c r="J37" s="70"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1806,6 +1840,9 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="O12" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
@@ -1813,8 +1850,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="S16" sqref="S16"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26:N32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1836,37 +1873,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="F1" s="84" t="s">
+      <c r="F1" s="57" t="s">
         <v>36</v>
       </c>
-      <c r="G1" s="85" t="s">
+      <c r="G1" s="58" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="F2" s="85"/>
-      <c r="G2" s="85" t="s">
+      <c r="F2" s="58"/>
+      <c r="G2" s="58" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8"/>
-      <c r="B4" s="35" t="s">
+      <c r="B4" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="35" t="s">
+      <c r="C4" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35" t="s">
+      <c r="D4" s="34"/>
+      <c r="E4" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35" t="s">
+      <c r="F4" s="34"/>
+      <c r="G4" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="35"/>
-      <c r="I4" s="35" t="s">
+      <c r="H4" s="34"/>
+      <c r="I4" s="34" t="s">
         <v>18</v>
       </c>
       <c r="J4" s="9"/>
@@ -1876,36 +1913,36 @@
       <c r="N4" s="2"/>
     </row>
     <row r="5" spans="1:14" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="37">
+      <c r="C5" s="36">
         <v>7500000</v>
       </c>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37">
+      <c r="D5" s="36"/>
+      <c r="E5" s="36">
         <v>9000000</v>
       </c>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37">
+      <c r="F5" s="36"/>
+      <c r="G5" s="36">
         <v>6500000</v>
       </c>
-      <c r="H5" s="37"/>
-      <c r="I5" s="37">
+      <c r="H5" s="36"/>
+      <c r="I5" s="36">
         <v>2500000</v>
       </c>
-      <c r="J5" s="38"/>
-      <c r="K5" s="39" t="s">
+      <c r="J5" s="37"/>
+      <c r="K5" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="L5" s="39"/>
-      <c r="M5" s="39" t="s">
+      <c r="L5" s="38"/>
+      <c r="M5" s="38" t="s">
         <v>21</v>
       </c>
       <c r="N5" s="2"/>
     </row>
     <row r="6" spans="1:14" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B6" s="38"/>
+      <c r="B6" s="37"/>
       <c r="C6" s="6" t="s">
         <v>22</v>
       </c>
@@ -1945,10 +1982,10 @@
     </row>
     <row r="7" spans="1:14" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A7" s="8"/>
-      <c r="B7" s="40" t="s">
+      <c r="B7" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="59">
+      <c r="C7" s="51">
         <v>80</v>
       </c>
       <c r="D7" s="3"/>
@@ -1964,12 +2001,12 @@
         <v>30</v>
       </c>
       <c r="J7" s="3"/>
-      <c r="K7" s="58">
+      <c r="K7" s="50">
         <f>AVERAGE(I7,G7,E7,C7)</f>
         <v>55</v>
       </c>
       <c r="L7" s="3"/>
-      <c r="M7" s="58">
+      <c r="M7" s="50">
         <v>100</v>
       </c>
       <c r="N7" s="3"/>
@@ -2006,15 +2043,15 @@
       <c r="J8" s="4">
         <v>0</v>
       </c>
-      <c r="K8" s="60">
+      <c r="K8" s="52">
         <f>AVERAGE(I8,G8,E8,C8)</f>
         <v>57</v>
       </c>
-      <c r="L8" s="61">
+      <c r="L8" s="53">
         <f>K8/K7 - 1</f>
         <v>3.6363636363636376E-2</v>
       </c>
-      <c r="M8" s="60">
+      <c r="M8" s="52">
         <f>($C$5*$C8+$E$5*$E8+$G$5*$G8+$I$5*$I8)/($C$7*$C$5+$E$7*$E$5+$G$7*$G$5+$I$7*$I$5)*100</f>
         <v>103.74414976599064</v>
       </c>
@@ -2024,7 +2061,7 @@
       </c>
     </row>
     <row r="9" spans="1:14" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B9" s="40" t="s">
+      <c r="B9" s="39" t="s">
         <v>26</v>
       </c>
       <c r="C9" s="1">
@@ -2055,7 +2092,7 @@
       <c r="J9" s="3">
         <v>0.1</v>
       </c>
-      <c r="K9" s="58">
+      <c r="K9" s="50">
         <f t="shared" ref="K9:K10" si="4">AVERAGE(I9,G9,E9,C9)</f>
         <v>57.75</v>
       </c>
@@ -2063,7 +2100,7 @@
         <f t="shared" ref="L9:L10" si="5">K9/K8 - 1</f>
         <v>1.3157894736842035E-2</v>
       </c>
-      <c r="M9" s="58">
+      <c r="M9" s="50">
         <f t="shared" ref="M9:M10" si="6">($C$5*$C9+$E$5*$E9+$G$5*$G9+$I$5*$I9)/($C$7*$C$5+$E$7*$E$5+$G$7*$G$5+$I$7*$I$5)*100</f>
         <v>104.21216848673947</v>
       </c>
@@ -2104,15 +2141,15 @@
       <c r="J10" s="4">
         <v>0</v>
       </c>
-      <c r="K10" s="60">
+      <c r="K10" s="52">
         <f t="shared" si="4"/>
         <v>58.375</v>
       </c>
-      <c r="L10" s="61">
+      <c r="L10" s="53">
         <f t="shared" si="5"/>
         <v>1.0822510822510845E-2</v>
       </c>
-      <c r="M10" s="60">
+      <c r="M10" s="52">
         <f t="shared" si="6"/>
         <v>105.22620904836192</v>
       </c>
@@ -2124,299 +2161,299 @@
     <row r="11" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B11" s="5"/>
       <c r="C11" s="8"/>
-      <c r="D11" s="62"/>
+      <c r="D11" s="54"/>
       <c r="E11" s="8"/>
-      <c r="F11" s="62"/>
+      <c r="F11" s="54"/>
       <c r="G11" s="8"/>
-      <c r="H11" s="62"/>
+      <c r="H11" s="54"/>
       <c r="I11" s="8"/>
-      <c r="J11" s="62"/>
-      <c r="K11" s="63"/>
-      <c r="L11" s="64"/>
-      <c r="M11" s="63"/>
-      <c r="N11" s="62"/>
+      <c r="J11" s="54"/>
+      <c r="K11" s="55"/>
+      <c r="L11" s="56"/>
+      <c r="M11" s="55"/>
+      <c r="N11" s="54"/>
     </row>
     <row r="12" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="68" t="s">
+      <c r="B12" s="62" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="77"/>
-      <c r="D12" s="77"/>
-      <c r="E12" s="77"/>
-      <c r="F12" s="77"/>
-      <c r="G12" s="77"/>
-      <c r="H12" s="77"/>
-      <c r="I12" s="77"/>
-      <c r="J12" s="77"/>
-      <c r="K12" s="77"/>
-      <c r="L12" s="77"/>
-      <c r="M12" s="77"/>
-      <c r="N12" s="78"/>
+      <c r="C12" s="71"/>
+      <c r="D12" s="71"/>
+      <c r="E12" s="71"/>
+      <c r="F12" s="71"/>
+      <c r="G12" s="71"/>
+      <c r="H12" s="71"/>
+      <c r="I12" s="71"/>
+      <c r="J12" s="71"/>
+      <c r="K12" s="71"/>
+      <c r="L12" s="71"/>
+      <c r="M12" s="71"/>
+      <c r="N12" s="72"/>
     </row>
     <row r="13" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="79"/>
-      <c r="C13" s="80"/>
-      <c r="D13" s="80"/>
-      <c r="E13" s="80"/>
-      <c r="F13" s="80"/>
-      <c r="G13" s="80"/>
-      <c r="H13" s="80"/>
-      <c r="I13" s="80"/>
-      <c r="J13" s="80"/>
-      <c r="K13" s="80"/>
-      <c r="L13" s="80"/>
-      <c r="M13" s="80"/>
-      <c r="N13" s="81"/>
+      <c r="B13" s="73"/>
+      <c r="C13" s="74"/>
+      <c r="D13" s="74"/>
+      <c r="E13" s="74"/>
+      <c r="F13" s="74"/>
+      <c r="G13" s="74"/>
+      <c r="H13" s="74"/>
+      <c r="I13" s="74"/>
+      <c r="J13" s="74"/>
+      <c r="K13" s="74"/>
+      <c r="L13" s="74"/>
+      <c r="M13" s="74"/>
+      <c r="N13" s="75"/>
     </row>
     <row r="14" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F14" s="34"/>
+      <c r="F14" s="33"/>
     </row>
     <row r="15" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="68" t="s">
+      <c r="B15" s="62" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="69"/>
-      <c r="D15" s="69"/>
-      <c r="E15" s="69"/>
-      <c r="F15" s="69"/>
-      <c r="G15" s="69"/>
-      <c r="H15" s="69"/>
-      <c r="I15" s="69"/>
-      <c r="J15" s="69"/>
-      <c r="K15" s="69"/>
-      <c r="L15" s="69"/>
-      <c r="M15" s="69"/>
-      <c r="N15" s="70"/>
+      <c r="C15" s="63"/>
+      <c r="D15" s="63"/>
+      <c r="E15" s="63"/>
+      <c r="F15" s="63"/>
+      <c r="G15" s="63"/>
+      <c r="H15" s="63"/>
+      <c r="I15" s="63"/>
+      <c r="J15" s="63"/>
+      <c r="K15" s="63"/>
+      <c r="L15" s="63"/>
+      <c r="M15" s="63"/>
+      <c r="N15" s="64"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B16" s="71"/>
-      <c r="C16" s="72"/>
-      <c r="D16" s="72"/>
-      <c r="E16" s="72"/>
-      <c r="F16" s="72"/>
-      <c r="G16" s="72"/>
-      <c r="H16" s="72"/>
-      <c r="I16" s="72"/>
-      <c r="J16" s="72"/>
-      <c r="K16" s="72"/>
-      <c r="L16" s="72"/>
-      <c r="M16" s="72"/>
-      <c r="N16" s="73"/>
+      <c r="B16" s="65"/>
+      <c r="C16" s="66"/>
+      <c r="D16" s="66"/>
+      <c r="E16" s="66"/>
+      <c r="F16" s="66"/>
+      <c r="G16" s="66"/>
+      <c r="H16" s="66"/>
+      <c r="I16" s="66"/>
+      <c r="J16" s="66"/>
+      <c r="K16" s="66"/>
+      <c r="L16" s="66"/>
+      <c r="M16" s="66"/>
+      <c r="N16" s="67"/>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B17" s="71"/>
-      <c r="C17" s="72"/>
-      <c r="D17" s="72"/>
-      <c r="E17" s="72"/>
-      <c r="F17" s="72"/>
-      <c r="G17" s="72"/>
-      <c r="H17" s="72"/>
-      <c r="I17" s="72"/>
-      <c r="J17" s="72"/>
-      <c r="K17" s="72"/>
-      <c r="L17" s="72"/>
-      <c r="M17" s="72"/>
-      <c r="N17" s="73"/>
+      <c r="B17" s="65"/>
+      <c r="C17" s="66"/>
+      <c r="D17" s="66"/>
+      <c r="E17" s="66"/>
+      <c r="F17" s="66"/>
+      <c r="G17" s="66"/>
+      <c r="H17" s="66"/>
+      <c r="I17" s="66"/>
+      <c r="J17" s="66"/>
+      <c r="K17" s="66"/>
+      <c r="L17" s="66"/>
+      <c r="M17" s="66"/>
+      <c r="N17" s="67"/>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B18" s="71"/>
-      <c r="C18" s="72"/>
-      <c r="D18" s="72"/>
-      <c r="E18" s="72"/>
-      <c r="F18" s="72"/>
-      <c r="G18" s="72"/>
-      <c r="H18" s="72"/>
-      <c r="I18" s="72"/>
-      <c r="J18" s="72"/>
-      <c r="K18" s="72"/>
-      <c r="L18" s="72"/>
-      <c r="M18" s="72"/>
-      <c r="N18" s="73"/>
+      <c r="B18" s="65"/>
+      <c r="C18" s="66"/>
+      <c r="D18" s="66"/>
+      <c r="E18" s="66"/>
+      <c r="F18" s="66"/>
+      <c r="G18" s="66"/>
+      <c r="H18" s="66"/>
+      <c r="I18" s="66"/>
+      <c r="J18" s="66"/>
+      <c r="K18" s="66"/>
+      <c r="L18" s="66"/>
+      <c r="M18" s="66"/>
+      <c r="N18" s="67"/>
     </row>
     <row r="19" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="74"/>
-      <c r="C19" s="75"/>
-      <c r="D19" s="75"/>
-      <c r="E19" s="75"/>
-      <c r="F19" s="75"/>
-      <c r="G19" s="75"/>
-      <c r="H19" s="75"/>
-      <c r="I19" s="75"/>
-      <c r="J19" s="75"/>
-      <c r="K19" s="75"/>
-      <c r="L19" s="75"/>
-      <c r="M19" s="75"/>
-      <c r="N19" s="76"/>
+      <c r="B19" s="68"/>
+      <c r="C19" s="69"/>
+      <c r="D19" s="69"/>
+      <c r="E19" s="69"/>
+      <c r="F19" s="69"/>
+      <c r="G19" s="69"/>
+      <c r="H19" s="69"/>
+      <c r="I19" s="69"/>
+      <c r="J19" s="69"/>
+      <c r="K19" s="69"/>
+      <c r="L19" s="69"/>
+      <c r="M19" s="69"/>
+      <c r="N19" s="70"/>
     </row>
     <row r="20" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="21" spans="2:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="68" t="s">
+      <c r="B21" s="62" t="s">
         <v>32</v>
       </c>
-      <c r="C21" s="69"/>
-      <c r="D21" s="69"/>
-      <c r="E21" s="69"/>
-      <c r="F21" s="69"/>
-      <c r="G21" s="69"/>
-      <c r="H21" s="69"/>
-      <c r="I21" s="69"/>
-      <c r="J21" s="69"/>
-      <c r="K21" s="69"/>
-      <c r="L21" s="69"/>
-      <c r="M21" s="69"/>
-      <c r="N21" s="70"/>
+      <c r="C21" s="63"/>
+      <c r="D21" s="63"/>
+      <c r="E21" s="63"/>
+      <c r="F21" s="63"/>
+      <c r="G21" s="63"/>
+      <c r="H21" s="63"/>
+      <c r="I21" s="63"/>
+      <c r="J21" s="63"/>
+      <c r="K21" s="63"/>
+      <c r="L21" s="63"/>
+      <c r="M21" s="63"/>
+      <c r="N21" s="64"/>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B22" s="71"/>
-      <c r="C22" s="72"/>
-      <c r="D22" s="72"/>
-      <c r="E22" s="72"/>
-      <c r="F22" s="72"/>
-      <c r="G22" s="72"/>
-      <c r="H22" s="72"/>
-      <c r="I22" s="72"/>
-      <c r="J22" s="72"/>
-      <c r="K22" s="72"/>
-      <c r="L22" s="72"/>
-      <c r="M22" s="72"/>
-      <c r="N22" s="73"/>
+      <c r="B22" s="65"/>
+      <c r="C22" s="66"/>
+      <c r="D22" s="66"/>
+      <c r="E22" s="66"/>
+      <c r="F22" s="66"/>
+      <c r="G22" s="66"/>
+      <c r="H22" s="66"/>
+      <c r="I22" s="66"/>
+      <c r="J22" s="66"/>
+      <c r="K22" s="66"/>
+      <c r="L22" s="66"/>
+      <c r="M22" s="66"/>
+      <c r="N22" s="67"/>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B23" s="71"/>
-      <c r="C23" s="72"/>
-      <c r="D23" s="72"/>
-      <c r="E23" s="72"/>
-      <c r="F23" s="72"/>
-      <c r="G23" s="72"/>
-      <c r="H23" s="72"/>
-      <c r="I23" s="72"/>
-      <c r="J23" s="72"/>
-      <c r="K23" s="72"/>
-      <c r="L23" s="72"/>
-      <c r="M23" s="72"/>
-      <c r="N23" s="73"/>
+      <c r="B23" s="65"/>
+      <c r="C23" s="66"/>
+      <c r="D23" s="66"/>
+      <c r="E23" s="66"/>
+      <c r="F23" s="66"/>
+      <c r="G23" s="66"/>
+      <c r="H23" s="66"/>
+      <c r="I23" s="66"/>
+      <c r="J23" s="66"/>
+      <c r="K23" s="66"/>
+      <c r="L23" s="66"/>
+      <c r="M23" s="66"/>
+      <c r="N23" s="67"/>
     </row>
     <row r="24" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="74"/>
-      <c r="C24" s="75"/>
-      <c r="D24" s="75"/>
-      <c r="E24" s="75"/>
-      <c r="F24" s="75"/>
-      <c r="G24" s="75"/>
-      <c r="H24" s="75"/>
-      <c r="I24" s="75"/>
-      <c r="J24" s="75"/>
-      <c r="K24" s="75"/>
-      <c r="L24" s="75"/>
-      <c r="M24" s="75"/>
-      <c r="N24" s="76"/>
+      <c r="B24" s="68"/>
+      <c r="C24" s="69"/>
+      <c r="D24" s="69"/>
+      <c r="E24" s="69"/>
+      <c r="F24" s="69"/>
+      <c r="G24" s="69"/>
+      <c r="H24" s="69"/>
+      <c r="I24" s="69"/>
+      <c r="J24" s="69"/>
+      <c r="K24" s="69"/>
+      <c r="L24" s="69"/>
+      <c r="M24" s="69"/>
+      <c r="N24" s="70"/>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B26" s="82" t="s">
+      <c r="B26" s="76" t="s">
         <v>33</v>
       </c>
-      <c r="C26" s="83"/>
-      <c r="D26" s="83"/>
-      <c r="E26" s="83"/>
-      <c r="F26" s="83"/>
-      <c r="G26" s="83"/>
-      <c r="H26" s="83"/>
-      <c r="I26" s="83"/>
-      <c r="J26" s="83"/>
-      <c r="K26" s="83"/>
-      <c r="L26" s="83"/>
-      <c r="M26" s="83"/>
-      <c r="N26" s="83"/>
+      <c r="C26" s="77"/>
+      <c r="D26" s="77"/>
+      <c r="E26" s="77"/>
+      <c r="F26" s="77"/>
+      <c r="G26" s="77"/>
+      <c r="H26" s="77"/>
+      <c r="I26" s="77"/>
+      <c r="J26" s="77"/>
+      <c r="K26" s="77"/>
+      <c r="L26" s="77"/>
+      <c r="M26" s="77"/>
+      <c r="N26" s="77"/>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B27" s="83"/>
-      <c r="C27" s="83"/>
-      <c r="D27" s="83"/>
-      <c r="E27" s="83"/>
-      <c r="F27" s="83"/>
-      <c r="G27" s="83"/>
-      <c r="H27" s="83"/>
-      <c r="I27" s="83"/>
-      <c r="J27" s="83"/>
-      <c r="K27" s="83"/>
-      <c r="L27" s="83"/>
-      <c r="M27" s="83"/>
-      <c r="N27" s="83"/>
+      <c r="B27" s="77"/>
+      <c r="C27" s="77"/>
+      <c r="D27" s="77"/>
+      <c r="E27" s="77"/>
+      <c r="F27" s="77"/>
+      <c r="G27" s="77"/>
+      <c r="H27" s="77"/>
+      <c r="I27" s="77"/>
+      <c r="J27" s="77"/>
+      <c r="K27" s="77"/>
+      <c r="L27" s="77"/>
+      <c r="M27" s="77"/>
+      <c r="N27" s="77"/>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B28" s="83"/>
-      <c r="C28" s="83"/>
-      <c r="D28" s="83"/>
-      <c r="E28" s="83"/>
-      <c r="F28" s="83"/>
-      <c r="G28" s="83"/>
-      <c r="H28" s="83"/>
-      <c r="I28" s="83"/>
-      <c r="J28" s="83"/>
-      <c r="K28" s="83"/>
-      <c r="L28" s="83"/>
-      <c r="M28" s="83"/>
-      <c r="N28" s="83"/>
+      <c r="B28" s="77"/>
+      <c r="C28" s="77"/>
+      <c r="D28" s="77"/>
+      <c r="E28" s="77"/>
+      <c r="F28" s="77"/>
+      <c r="G28" s="77"/>
+      <c r="H28" s="77"/>
+      <c r="I28" s="77"/>
+      <c r="J28" s="77"/>
+      <c r="K28" s="77"/>
+      <c r="L28" s="77"/>
+      <c r="M28" s="77"/>
+      <c r="N28" s="77"/>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B29" s="83"/>
-      <c r="C29" s="83"/>
-      <c r="D29" s="83"/>
-      <c r="E29" s="83"/>
-      <c r="F29" s="83"/>
-      <c r="G29" s="83"/>
-      <c r="H29" s="83"/>
-      <c r="I29" s="83"/>
-      <c r="J29" s="83"/>
-      <c r="K29" s="83"/>
-      <c r="L29" s="83"/>
-      <c r="M29" s="83"/>
-      <c r="N29" s="83"/>
+      <c r="B29" s="77"/>
+      <c r="C29" s="77"/>
+      <c r="D29" s="77"/>
+      <c r="E29" s="77"/>
+      <c r="F29" s="77"/>
+      <c r="G29" s="77"/>
+      <c r="H29" s="77"/>
+      <c r="I29" s="77"/>
+      <c r="J29" s="77"/>
+      <c r="K29" s="77"/>
+      <c r="L29" s="77"/>
+      <c r="M29" s="77"/>
+      <c r="N29" s="77"/>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B30" s="83"/>
-      <c r="C30" s="83"/>
-      <c r="D30" s="83"/>
-      <c r="E30" s="83"/>
-      <c r="F30" s="83"/>
-      <c r="G30" s="83"/>
-      <c r="H30" s="83"/>
-      <c r="I30" s="83"/>
-      <c r="J30" s="83"/>
-      <c r="K30" s="83"/>
-      <c r="L30" s="83"/>
-      <c r="M30" s="83"/>
-      <c r="N30" s="83"/>
+      <c r="B30" s="77"/>
+      <c r="C30" s="77"/>
+      <c r="D30" s="77"/>
+      <c r="E30" s="77"/>
+      <c r="F30" s="77"/>
+      <c r="G30" s="77"/>
+      <c r="H30" s="77"/>
+      <c r="I30" s="77"/>
+      <c r="J30" s="77"/>
+      <c r="K30" s="77"/>
+      <c r="L30" s="77"/>
+      <c r="M30" s="77"/>
+      <c r="N30" s="77"/>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B31" s="83"/>
-      <c r="C31" s="83"/>
-      <c r="D31" s="83"/>
-      <c r="E31" s="83"/>
-      <c r="F31" s="83"/>
-      <c r="G31" s="83"/>
-      <c r="H31" s="83"/>
-      <c r="I31" s="83"/>
-      <c r="J31" s="83"/>
-      <c r="K31" s="83"/>
-      <c r="L31" s="83"/>
-      <c r="M31" s="83"/>
-      <c r="N31" s="83"/>
+      <c r="B31" s="77"/>
+      <c r="C31" s="77"/>
+      <c r="D31" s="77"/>
+      <c r="E31" s="77"/>
+      <c r="F31" s="77"/>
+      <c r="G31" s="77"/>
+      <c r="H31" s="77"/>
+      <c r="I31" s="77"/>
+      <c r="J31" s="77"/>
+      <c r="K31" s="77"/>
+      <c r="L31" s="77"/>
+      <c r="M31" s="77"/>
+      <c r="N31" s="77"/>
     </row>
     <row r="32" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B32" s="83"/>
-      <c r="C32" s="83"/>
-      <c r="D32" s="83"/>
-      <c r="E32" s="83"/>
-      <c r="F32" s="83"/>
-      <c r="G32" s="83"/>
-      <c r="H32" s="83"/>
-      <c r="I32" s="83"/>
-      <c r="J32" s="83"/>
-      <c r="K32" s="83"/>
-      <c r="L32" s="83"/>
-      <c r="M32" s="83"/>
-      <c r="N32" s="83"/>
+      <c r="B32" s="77"/>
+      <c r="C32" s="77"/>
+      <c r="D32" s="77"/>
+      <c r="E32" s="77"/>
+      <c r="F32" s="77"/>
+      <c r="G32" s="77"/>
+      <c r="H32" s="77"/>
+      <c r="I32" s="77"/>
+      <c r="J32" s="77"/>
+      <c r="K32" s="77"/>
+      <c r="L32" s="77"/>
+      <c r="M32" s="77"/>
+      <c r="N32" s="77"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>